<commit_message>
trying to run this shit
</commit_message>
<xml_diff>
--- a/target/classes/Monster.xlsx
+++ b/target/classes/Monster.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hossein Mohammadi\Desktop\jadid\main\src\main\java\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hossein Mohammadi\Desktop\AP PROJECT MOLAYEE\project-team-45\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="116">
   <si>
     <t>Name</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Battle OX</t>
-  </si>
-  <si>
-    <t>EARHT</t>
   </si>
   <si>
     <t>Beast-Warrior</t>
@@ -1182,7 +1179,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1223,13 +1222,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
       </c>
       <c r="F2">
         <v>1700</v>
@@ -1238,7 +1237,7 @@
         <v>1000</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2">
         <v>2900</v>
@@ -1246,19 +1245,19 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3">
         <v>1700</v>
@@ -1267,7 +1266,7 @@
         <v>1150</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I3">
         <v>3100</v>
@@ -1275,19 +1274,19 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
       </c>
       <c r="F4">
         <v>800</v>
@@ -1296,7 +1295,7 @@
         <v>1400</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4">
         <v>1700</v>
@@ -1304,19 +1303,19 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5">
         <v>1300</v>
@@ -1325,7 +1324,7 @@
         <v>1000</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I5">
         <v>2500</v>
@@ -1333,19 +1332,19 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6">
         <v>1200</v>
@@ -1354,7 +1353,7 @@
         <v>800</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I6">
         <v>1700</v>
@@ -1362,19 +1361,19 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7">
         <v>7</v>
       </c>
       <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
       </c>
       <c r="F7">
         <v>2500</v>
@@ -1383,7 +1382,7 @@
         <v>2400</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I7">
         <v>8700</v>
@@ -1391,19 +1390,19 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" t="s">
-        <v>34</v>
-      </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8">
         <v>1300</v>
@@ -1412,7 +1411,7 @@
         <v>1000</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I8">
         <v>2500</v>
@@ -1420,19 +1419,19 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9">
         <v>600</v>
@@ -1441,7 +1440,7 @@
         <v>500</v>
       </c>
       <c r="H9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I9">
         <v>700</v>
@@ -1449,19 +1448,19 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
       <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10">
         <v>1300</v>
@@ -1470,7 +1469,7 @@
         <v>1400</v>
       </c>
       <c r="H10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I10">
         <v>2800</v>
@@ -1478,19 +1477,19 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11">
         <v>2500</v>
@@ -1499,7 +1498,7 @@
         <v>2100</v>
       </c>
       <c r="H11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I11">
         <v>8300</v>
@@ -1507,19 +1506,19 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12">
         <v>3</v>
       </c>
       <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="D12" t="s">
-        <v>45</v>
-      </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12">
         <v>1000</v>
@@ -1528,7 +1527,7 @@
         <v>500</v>
       </c>
       <c r="H12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I12">
         <v>1300</v>
@@ -1536,19 +1535,19 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
         <v>48</v>
       </c>
-      <c r="D13" t="s">
-        <v>49</v>
-      </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13">
         <v>1200</v>
@@ -1557,7 +1556,7 @@
         <v>700</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I13">
         <v>1600</v>
@@ -1565,19 +1564,19 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14">
         <v>1100</v>
@@ -1586,7 +1585,7 @@
         <v>1000</v>
       </c>
       <c r="H14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I14">
         <v>1700</v>
@@ -1594,19 +1593,19 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15">
         <v>700</v>
@@ -1615,7 +1614,7 @@
         <v>1000</v>
       </c>
       <c r="H15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I15">
         <v>1300</v>
@@ -1623,19 +1622,19 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16">
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F16">
         <v>1600</v>
@@ -1644,7 +1643,7 @@
         <v>1400</v>
       </c>
       <c r="H16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I16">
         <v>3900</v>
@@ -1652,19 +1651,19 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17">
         <v>900</v>
@@ -1673,7 +1672,7 @@
         <v>1000</v>
       </c>
       <c r="H17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I17">
         <v>1500</v>
@@ -1681,19 +1680,19 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F18">
         <v>3000</v>
@@ -1702,7 +1701,7 @@
         <v>2500</v>
       </c>
       <c r="H18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I18">
         <v>11300</v>
@@ -1710,19 +1709,19 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19">
         <v>8</v>
       </c>
       <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
         <v>18</v>
       </c>
-      <c r="D19" t="s">
-        <v>19</v>
-      </c>
       <c r="E19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F19">
         <v>2550</v>
@@ -1731,7 +1730,7 @@
         <v>2500</v>
       </c>
       <c r="H19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I19">
         <v>10200</v>
@@ -1739,19 +1738,19 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F20">
         <v>2050</v>
@@ -1760,7 +1759,7 @@
         <v>2500</v>
       </c>
       <c r="H20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I20">
         <v>7900</v>
@@ -1768,19 +1767,19 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21">
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F21">
         <v>2000</v>
@@ -1789,7 +1788,7 @@
         <v>2300</v>
       </c>
       <c r="H21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I21">
         <v>7500</v>
@@ -1797,19 +1796,19 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F22">
         <v>500</v>
@@ -1818,7 +1817,7 @@
         <v>500</v>
       </c>
       <c r="H22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I22">
         <v>600</v>
@@ -1826,19 +1825,19 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F23">
         <v>450</v>
@@ -1847,7 +1846,7 @@
         <v>600</v>
       </c>
       <c r="H23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I23">
         <v>600</v>
@@ -1855,19 +1854,19 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B24">
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F24">
         <v>3750</v>
@@ -1876,7 +1875,7 @@
         <v>3400</v>
       </c>
       <c r="H24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I24">
         <v>20000</v>
@@ -1884,19 +1883,19 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1905,7 +1904,7 @@
         <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I25">
         <v>8000</v>
@@ -1913,19 +1912,19 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F26">
         <v>200</v>
@@ -1934,7 +1933,7 @@
         <v>2000</v>
       </c>
       <c r="H26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I26">
         <v>1000</v>
@@ -1942,19 +1941,19 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B27">
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F27">
         <v>300</v>
@@ -1963,7 +1962,7 @@
         <v>500</v>
       </c>
       <c r="H27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I27">
         <v>700</v>
@@ -1971,19 +1970,19 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B28">
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F28">
         <v>3000</v>
@@ -1992,7 +1991,7 @@
         <v>1200</v>
       </c>
       <c r="H28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I28">
         <v>9200</v>
@@ -2000,19 +1999,19 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F29">
         <v>100</v>
@@ -2021,7 +2020,7 @@
         <v>100</v>
       </c>
       <c r="H29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I29">
         <v>200</v>
@@ -2029,19 +2028,19 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B30">
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F30">
         <v>2000</v>
@@ -2050,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="H30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I30">
         <v>2500</v>
@@ -2058,19 +2057,19 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
       <c r="C31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" t="s">
         <v>44</v>
       </c>
-      <c r="D31" t="s">
-        <v>45</v>
-      </c>
       <c r="E31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -2079,7 +2078,7 @@
         <v>0</v>
       </c>
       <c r="H31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I31">
         <v>8000</v>
@@ -2087,19 +2086,19 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B32">
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F32">
         <v>2000</v>
@@ -2108,7 +2107,7 @@
         <v>100</v>
       </c>
       <c r="H32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I32">
         <v>2600</v>
@@ -2116,19 +2115,19 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B33">
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F33">
         <v>1600</v>
@@ -2137,7 +2136,7 @@
         <v>600</v>
       </c>
       <c r="H33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I33">
         <v>2500</v>
@@ -2145,19 +2144,19 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B34">
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F34">
         <v>1800</v>
@@ -2166,7 +2165,7 @@
         <v>600</v>
       </c>
       <c r="H34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I34">
         <v>2700</v>
@@ -2174,19 +2173,19 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B35">
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F35">
         <v>1000</v>
@@ -2195,7 +2194,7 @@
         <v>0</v>
       </c>
       <c r="H35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I35">
         <v>1000</v>
@@ -2203,19 +2202,19 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B36">
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F36">
         <v>1700</v>
@@ -2224,7 +2223,7 @@
         <v>1600</v>
       </c>
       <c r="H36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I36">
         <v>3400</v>
@@ -2232,19 +2231,19 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B37">
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F37">
         <v>1800</v>
@@ -2253,27 +2252,27 @@
         <v>1500</v>
       </c>
       <c r="H37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I37">
         <v>3500</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B38">
         <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F38">
         <v>2500</v>
@@ -2282,7 +2281,7 @@
         <v>1000</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I38">
         <v>5800</v>
@@ -2290,19 +2289,19 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B39">
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F39">
         <v>1800</v>
@@ -2311,7 +2310,7 @@
         <v>1200</v>
       </c>
       <c r="H39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I39">
         <v>3200</v>
@@ -2319,19 +2318,19 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B40">
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F40">
         <v>2000</v>
@@ -2340,7 +2339,7 @@
         <v>1200</v>
       </c>
       <c r="H40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I40">
         <v>4300</v>
@@ -2348,19 +2347,19 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B41">
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F41">
         <v>2900</v>
@@ -2369,7 +2368,7 @@
         <v>2900</v>
       </c>
       <c r="H41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I41">
         <v>11700</v>
@@ -2377,19 +2376,19 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B42">
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F42">
         <v>1000</v>
@@ -2398,7 +2397,7 @@
         <v>1000</v>
       </c>
       <c r="H42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I42">
         <v>2100</v>

</xml_diff>